<commit_message>
rajouté une arborescence, rationalilsé l'optimisation de la taille en mémoire, ajouté affichage interactif plus compact (dernière version avant splittage de P3_Cleaning).
</commit_message>
<xml_diff>
--- a/energy data.xlsx
+++ b/energy data.xlsx
@@ -626,7 +626,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +676,7 @@
         <v>4.1840000000000002</v>
       </c>
       <c r="D5" s="2">
-        <f>E5*1000</f>
+        <f t="shared" ref="D5:D12" si="0">E5*1000</f>
         <v>1000</v>
       </c>
       <c r="E5" s="14">
@@ -700,7 +700,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="15">
-        <f>E6*$B$5</f>
+        <f t="shared" ref="B6:B12" si="1">E6*$B$5</f>
         <v>16736</v>
       </c>
       <c r="C6" s="12">
@@ -708,7 +708,7 @@
         <v>16.736000000000001</v>
       </c>
       <c r="D6" s="12">
-        <f>E6*1000</f>
+        <f t="shared" si="0"/>
         <v>4000</v>
       </c>
       <c r="E6" s="13">
@@ -732,30 +732,30 @@
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <f>E7*$B$5</f>
+        <f t="shared" si="1"/>
         <v>16736</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" ref="C7:C12" si="0">E7*$C$5</f>
+        <f t="shared" ref="C7:C12" si="2">E7*$C$5</f>
         <v>16.736000000000001</v>
       </c>
       <c r="D7" s="4">
-        <f>E7*1000</f>
+        <f t="shared" si="0"/>
         <v>4000</v>
       </c>
       <c r="E7" s="16">
         <v>4</v>
       </c>
       <c r="F7" s="21">
-        <f t="shared" ref="F7:F12" si="1">F6*$E$6</f>
+        <f t="shared" ref="F7:F12" si="3">F6*$E$6</f>
         <v>6694.4000000000005</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" ref="G7:G12" si="2">E7*$G$5</f>
+        <f t="shared" ref="G7:G12" si="4">E7*$G$5</f>
         <v>400000</v>
       </c>
       <c r="H7" s="26">
-        <f t="shared" ref="H7:H12" si="3">E7*$H$5</f>
+        <f t="shared" ref="H7:H12" si="5">E7*$H$5</f>
         <v>400</v>
       </c>
     </row>
@@ -764,30 +764,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="3">
-        <f>E8*$B$5</f>
+        <f t="shared" si="1"/>
         <v>37656</v>
       </c>
       <c r="C8" s="4">
+        <f t="shared" si="2"/>
+        <v>37.655999999999999</v>
+      </c>
+      <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>37.655999999999999</v>
-      </c>
-      <c r="D8" s="4">
-        <f>E8*1000</f>
         <v>9000</v>
       </c>
       <c r="E8" s="16">
         <v>9</v>
       </c>
       <c r="F8" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>26777.600000000002</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>900000</v>
       </c>
       <c r="H8" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>900</v>
       </c>
     </row>
@@ -796,30 +796,30 @@
         <v>5</v>
       </c>
       <c r="B9" s="3">
-        <f>E9*$B$5</f>
+        <f t="shared" si="1"/>
         <v>29288</v>
       </c>
       <c r="C9" s="4">
+        <f t="shared" si="2"/>
+        <v>29.288</v>
+      </c>
+      <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>29.288</v>
-      </c>
-      <c r="D9" s="4">
-        <f>E9*1000</f>
         <v>7000</v>
       </c>
       <c r="E9" s="16">
         <v>7</v>
       </c>
       <c r="F9" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>107110.40000000001</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>700000</v>
       </c>
       <c r="H9" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>700</v>
       </c>
     </row>
@@ -828,30 +828,30 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <f>E10*$B$5</f>
+        <f t="shared" si="1"/>
         <v>12552</v>
       </c>
       <c r="C10" s="4">
+        <f t="shared" si="2"/>
+        <v>12.552</v>
+      </c>
+      <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>12.552</v>
-      </c>
-      <c r="D10" s="4">
-        <f>E10*1000</f>
         <v>3000</v>
       </c>
       <c r="E10" s="16">
         <v>3</v>
       </c>
       <c r="F10" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>428441.60000000003</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>300000</v>
       </c>
       <c r="H10" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>300</v>
       </c>
     </row>
@@ -860,30 +860,30 @@
         <v>7</v>
       </c>
       <c r="B11" s="3">
-        <f>E11*$B$5</f>
+        <f t="shared" si="1"/>
         <v>10041.6</v>
       </c>
       <c r="C11" s="4">
+        <f t="shared" si="2"/>
+        <v>10.041600000000001</v>
+      </c>
+      <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>10.041600000000001</v>
-      </c>
-      <c r="D11" s="4">
-        <f>E11*1000</f>
         <v>2400</v>
       </c>
       <c r="E11" s="16">
         <v>2.4</v>
       </c>
       <c r="F11" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1713766.4000000001</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>240000</v>
       </c>
       <c r="H11" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>240</v>
       </c>
     </row>
@@ -892,30 +892,30 @@
         <v>8</v>
       </c>
       <c r="B12" s="5">
-        <f>E12*$B$5</f>
+        <f t="shared" si="1"/>
         <v>7949.5999999999995</v>
       </c>
       <c r="C12" s="6">
+        <f t="shared" si="2"/>
+        <v>7.9496000000000002</v>
+      </c>
+      <c r="D12" s="6">
         <f t="shared" si="0"/>
-        <v>7.9496000000000002</v>
-      </c>
-      <c r="D12" s="6">
-        <f>E12*1000</f>
         <v>1900</v>
       </c>
       <c r="E12" s="17">
         <v>1.9</v>
       </c>
       <c r="F12" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6855065.6000000006</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>190000</v>
       </c>
       <c r="H12" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
partie 1.4 : condition 2 calcul de l'energie à partir de la composition, remplissage des valeurs manquantes OK, vérification des valeurs originales par comparaison avec les valeurs calculées en cours - partie 1.5 à relire
</commit_message>
<xml_diff>
--- a/energy data.xlsx
+++ b/energy data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>kcal/100g</t>
   </si>
@@ -27,9 +27,6 @@
     <t>protides</t>
   </si>
   <si>
-    <t>gluclides</t>
-  </si>
-  <si>
     <t>lipides</t>
   </si>
   <si>
@@ -61,6 +58,36 @@
   </si>
   <si>
     <t>*source : « The Food Labelling Regulations 1996 » [archive], sur www.legislation.gov.uk (consulté le 11 janvier 2017) cité dans Wikipédia</t>
+  </si>
+  <si>
+    <t>1kcal</t>
+  </si>
+  <si>
+    <t>glucides</t>
+  </si>
+  <si>
+    <t>swifter</t>
+  </si>
+  <si>
+    <t>sans</t>
+  </si>
+  <si>
+    <t>npartitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tous nuls : , </t>
+  </si>
+  <si>
+    <t xml:space="preserve">au moins un remplis : </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> partiellement rempli :  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tous remplis :  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplis et pas remplis : </t>
   </si>
 </sst>
 </file>
@@ -84,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,8 +124,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -188,47 +227,10 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color rgb="FFFF0000"/>
       </left>
       <right style="medium">
-        <color rgb="FFFF0000"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
         <color rgb="FFFF0000"/>
@@ -242,14 +244,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,9 +273,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -292,9 +285,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -307,9 +297,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -319,9 +306,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,6 +323,348 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16362839020122485"/>
+          <c:y val="6.0370684433676561E-2"/>
+          <c:w val="0.75072572178477692"/>
+          <c:h val="0.75169172035313769"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>apply</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil2!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil2!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>28.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.733333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>swifter.apply</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil2!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil2!$G$3:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>45.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="157899520"/>
+        <c:axId val="157898944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="157899520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4500000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Nb de lignes (millions)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="157898944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="157898944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>temps de calcul par ligne (µs)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.7049650043744535E-2"/>
+              <c:y val="7.279079345851E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="157899520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.58094356955380577"/>
+          <c:y val="5.3753621706377611E-2"/>
+          <c:w val="0.34127865266841645"/>
+          <c:h val="0.13058799468248286"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,300 +954,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="7"/>
-    <col min="4" max="5" width="11.42578125" style="7"/>
-    <col min="7" max="8" width="11.42578125" style="7"/>
+    <col min="2" max="2" width="11.42578125" style="5"/>
+    <col min="4" max="5" width="11.42578125" style="5"/>
+    <col min="7" max="8" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+      <c r="B5" s="12">
         <f>4184*E5</f>
         <v>4184</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="10">
         <f>B5/1000</f>
         <v>4.1840000000000002</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="10">
         <f t="shared" ref="D5:D12" si="0">E5*1000</f>
         <v>1000</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="11">
         <v>1</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="16">
         <f>C5*100</f>
         <v>418.40000000000003</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="10">
         <f>D5*100</f>
         <v>100000</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="20">
         <f>E5*100</f>
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <f t="shared" ref="B6:B12" si="1">E6*$B$5</f>
         <v>16736</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <f>E6*$C$5</f>
         <v>16.736000000000001</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="11">
         <v>4</v>
       </c>
-      <c r="F6" s="20">
-        <f>F5*$E$6</f>
+      <c r="F6" s="16">
+        <f>$F$5*E6</f>
         <v>1673.6000000000001</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="10">
         <f>E6*$G$5</f>
         <v>400000</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="20">
         <f>E6*$H$5</f>
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
         <f t="shared" si="1"/>
         <v>16736</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <f t="shared" ref="C7:C12" si="2">E7*$C$5</f>
         <v>16.736000000000001</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>4</v>
       </c>
-      <c r="F7" s="21">
-        <f t="shared" ref="F7:F12" si="3">F6*$E$6</f>
-        <v>6694.4000000000005</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="F7" s="17">
+        <f t="shared" ref="F7:F12" si="3">$F$5*E7</f>
+        <v>1673.6000000000001</v>
+      </c>
+      <c r="G7" s="2">
         <f t="shared" ref="G7:G12" si="4">E7*$G$5</f>
         <v>400000</v>
       </c>
-      <c r="H7" s="26">
-        <f t="shared" ref="H7:H12" si="5">E7*$H$5</f>
+      <c r="H7" s="21">
+        <f>E7*$H$5</f>
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
         <f t="shared" si="1"/>
         <v>37656</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <f t="shared" si="2"/>
         <v>37.655999999999999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>9000</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="13">
         <v>9</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="17">
         <f t="shared" si="3"/>
-        <v>26777.600000000002</v>
-      </c>
-      <c r="G8" s="4">
+        <v>3765.6000000000004</v>
+      </c>
+      <c r="G8" s="2">
         <f t="shared" si="4"/>
         <v>900000</v>
       </c>
-      <c r="H8" s="28">
-        <f t="shared" si="5"/>
+      <c r="H8" s="23">
+        <f t="shared" ref="H7:H12" si="5">E8*$H$5</f>
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
         <f t="shared" si="1"/>
         <v>29288</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <f t="shared" si="2"/>
         <v>29.288</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>7000</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <v>7</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="17">
         <f t="shared" si="3"/>
-        <v>107110.40000000001</v>
-      </c>
-      <c r="G9" s="4">
+        <v>2928.8</v>
+      </c>
+      <c r="G9" s="2">
         <f t="shared" si="4"/>
         <v>700000</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="21">
         <f t="shared" si="5"/>
         <v>700</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
         <f t="shared" si="1"/>
         <v>12552</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2">
         <f t="shared" si="2"/>
         <v>12.552</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <v>3</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="17">
         <f t="shared" si="3"/>
-        <v>428441.60000000003</v>
-      </c>
-      <c r="G10" s="4">
+        <v>1255.2</v>
+      </c>
+      <c r="G10" s="2">
         <f t="shared" si="4"/>
         <v>300000</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="21">
         <f t="shared" si="5"/>
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
         <f t="shared" si="1"/>
         <v>10041.6</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="2">
         <f t="shared" si="2"/>
         <v>10.041600000000001</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <v>2.4</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="17">
         <f t="shared" si="3"/>
-        <v>1713766.4000000001</v>
-      </c>
-      <c r="G11" s="4">
+        <v>1004.1600000000001</v>
+      </c>
+      <c r="G11" s="2">
         <f t="shared" si="4"/>
         <v>240000</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="21">
         <f t="shared" si="5"/>
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="5">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3">
         <f t="shared" si="1"/>
         <v>7949.5999999999995</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <f t="shared" si="2"/>
         <v>7.9496000000000002</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="14">
         <v>1.9</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="18">
         <f t="shared" si="3"/>
-        <v>6855065.6000000006</v>
-      </c>
-      <c r="G12" s="6">
+        <v>794.96</v>
+      </c>
+      <c r="G12" s="4">
         <f t="shared" si="4"/>
         <v>190000</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="22">
         <f t="shared" si="5"/>
         <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15">
+        <v>258749</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="24">
+        <v>1100158</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17">
+        <v>9524</v>
+      </c>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="25">
+        <v>1090634</v>
+      </c>
+    </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19">
+        <v>1358907</v>
       </c>
     </row>
   </sheetData>
@@ -927,13 +1301,192 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C2:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>25000</v>
+      </c>
+      <c r="D3">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="E3">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F3">
+        <f>D3*1000000/$C3</f>
+        <v>28.92</v>
+      </c>
+      <c r="G3">
+        <f>E3*1000000/$C3</f>
+        <v>45.6</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>250000</v>
+      </c>
+      <c r="D4">
+        <v>7.37</v>
+      </c>
+      <c r="E4">
+        <v>12.1</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F10" si="0">D4*1000000/$C4</f>
+        <v>29.48</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G10" si="1">E4*1000000/$C4</f>
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>500000</v>
+      </c>
+      <c r="D5">
+        <v>13.4</v>
+      </c>
+      <c r="E5">
+        <v>14.6</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>26.8</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>750000</v>
+      </c>
+      <c r="D6">
+        <v>20.8</v>
+      </c>
+      <c r="E6">
+        <v>18.5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>27.733333333333334</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>24.666666666666668</v>
+      </c>
+      <c r="H6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1000000</v>
+      </c>
+      <c r="D7">
+        <v>27.4</v>
+      </c>
+      <c r="E7">
+        <v>21.8</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>27.4</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1500000</v>
+      </c>
+      <c r="D8">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="E8">
+        <v>29.5</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>26.8</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>19.666666666666668</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2000000</v>
+      </c>
+      <c r="D9">
+        <v>55.8</v>
+      </c>
+      <c r="E9">
+        <v>37.6</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>27.9</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>4000000</v>
+      </c>
+      <c r="D10">
+        <v>113</v>
+      </c>
+      <c r="E10">
+        <v>62</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>28.25</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>15.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Grand ménage - réordonné les parties et mis à jour le 'Notebook_Content.txt ' - rappatrié presque tout le code dans P3_Cleaning_1 - crée une partie 'dealing with missing or erroneous data' pour alléger la partie finale 'Dropping rows' - réparé un pbe dans 'Dealing with Duplicates' - fonctionne sauf 2.4 à 2.6 à finir
</commit_message>
<xml_diff>
--- a/energy data.xlsx
+++ b/energy data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>kcal/100g</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t xml:space="preserve">remplis et pas remplis : </t>
+  </si>
+  <si>
+    <t>3500kcal max par jour</t>
   </si>
 </sst>
 </file>
@@ -511,11 +514,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="157899520"/>
-        <c:axId val="157898944"/>
+        <c:axId val="606386368"/>
+        <c:axId val="606386944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="157899520"/>
+        <c:axId val="606386368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4500000"/>
@@ -539,14 +542,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157898944"/>
+        <c:crossAx val="606386944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -554,7 +556,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="157898944"/>
+        <c:axId val="606386944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -591,7 +593,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157899520"/>
+        <c:crossAx val="606386368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -954,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,13 +970,13 @@
     <col min="7" max="8" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
@@ -996,8 +998,11 @@
       <c r="H4" s="19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1029,7 +1034,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1061,7 +1066,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -1093,7 +1098,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
@@ -1121,11 +1126,11 @@
         <v>900000</v>
       </c>
       <c r="H8" s="23">
-        <f t="shared" ref="H7:H12" si="5">E8*$H$5</f>
+        <f t="shared" ref="H8:H12" si="5">E8*$H$5</f>
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
@@ -1157,7 +1162,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
@@ -1189,7 +1194,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +1226,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
@@ -1253,7 +1258,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1261,7 +1266,7 @@
         <v>258749</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G16" s="5" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Fonctionne bien jusqu'à 2.5 (energy), reste encore à choisir si energy est en kcal ou kj - entamé le codage de 2.6 (nutriscore) - supprimé P3_Cleaning - vidé le fichier requirements
</commit_message>
<xml_diff>
--- a/energy data.xlsx
+++ b/energy data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>kcal/100g</t>
   </si>
@@ -66,15 +66,6 @@
     <t>glucides</t>
   </si>
   <si>
-    <t>swifter</t>
-  </si>
-  <si>
-    <t>sans</t>
-  </si>
-  <si>
-    <t>npartitions</t>
-  </si>
-  <si>
     <t xml:space="preserve">tous nuls : , </t>
   </si>
   <si>
@@ -91,13 +82,55 @@
   </si>
   <si>
     <t>3500kcal max par jour</t>
+  </si>
+  <si>
+    <t>energy-kj_100g</t>
+  </si>
+  <si>
+    <t>energy-kcal_100g</t>
+  </si>
+  <si>
+    <t>energy_100g</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Only kcal -&gt; vérifier si valable, sinon prendre calc-kcal</t>
+  </si>
+  <si>
+    <t>all nan -&gt; remplacer par calc</t>
+  </si>
+  <si>
+    <t>Only kj -&gt; vérifier si valable, sinon prendre calc-j</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> semble indiquer que energy_100g est calculé</t>
+  </si>
+  <si>
+    <t>OK 1</t>
+  </si>
+  <si>
+    <t>OK 2</t>
+  </si>
+  <si>
+    <t>OK 3</t>
+  </si>
+  <si>
+    <t>OK 3bis</t>
+  </si>
+  <si>
+    <t>OK 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +146,68 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,8 +232,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -243,11 +372,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,6 +458,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -326,347 +487,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.16362839020122485"/>
-          <c:y val="6.0370684433676561E-2"/>
-          <c:w val="0.75072572178477692"/>
-          <c:h val="0.75169172035313769"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>apply</c:v>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Feuil2!$C$3:$C$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>25000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>250000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>750000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Feuil2!$F$3:$F$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>28.92</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29.48</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>27.733333333333334</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>27.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>27.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>28.25</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>swifter.apply</c:v>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Feuil2!$C$3:$C$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>25000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>250000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>750000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Feuil2!$G$3:$G$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>45.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>48.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>29.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24.666666666666668</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21.8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19.666666666666668</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>18.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>15.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="606386368"/>
-        <c:axId val="606386944"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="606386368"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="4500000"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="fr-FR"/>
-                  <a:t>Nb de lignes (millions)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="606386944"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:dispUnits>
-          <c:builtInUnit val="millions"/>
-        </c:dispUnits>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="606386944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="fr-FR"/>
-                  <a:t>temps de calcul par ligne (µs)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="1.7049650043744535E-2"/>
-              <c:y val="7.279079345851E-2"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="606386368"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.58094356955380577"/>
-          <c:y val="5.3753621706377611E-2"/>
-          <c:w val="0.34127865266841645"/>
-          <c:h val="0.13058799468248286"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1400"/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -958,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1260,7 +1080,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G15" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I15">
         <v>258749</v>
@@ -1268,7 +1088,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G16" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I16" s="24">
         <v>1100158</v>
@@ -1276,7 +1096,7 @@
     </row>
     <row r="17" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G17" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I17">
         <v>9524</v>
@@ -1284,7 +1104,7 @@
     </row>
     <row r="18" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G18" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I18" s="25">
         <v>1090634</v>
@@ -1292,7 +1112,7 @@
     </row>
     <row r="19" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G19" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I19">
         <v>1358907</v>
@@ -1306,192 +1126,192 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:H10"/>
+  <dimension ref="A4:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="26"/>
+    <col min="2" max="2" width="17.7109375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="26" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="26"/>
+    <col min="6" max="6" width="4.28515625" style="26" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="26"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>25000</v>
-      </c>
-      <c r="D3">
-        <v>0.72299999999999998</v>
-      </c>
-      <c r="E3">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="F3">
-        <f>D3*1000000/$C3</f>
-        <v>28.92</v>
-      </c>
-      <c r="G3">
-        <f>E3*1000000/$C3</f>
-        <v>45.6</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>250000</v>
-      </c>
-      <c r="D4">
-        <v>7.37</v>
-      </c>
-      <c r="E4">
-        <v>12.1</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F10" si="0">D4*1000000/$C4</f>
-        <v>29.48</v>
-      </c>
-      <c r="G4">
-        <f t="shared" ref="G4:G10" si="1">E4*1000000/$C4</f>
-        <v>48.4</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>500000</v>
-      </c>
-      <c r="D5">
-        <v>13.4</v>
-      </c>
-      <c r="E5">
-        <v>14.6</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>26.8</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="1"/>
-        <v>29.2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>750000</v>
-      </c>
-      <c r="D6">
-        <v>20.8</v>
-      </c>
-      <c r="E6">
-        <v>18.5</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>27.733333333333334</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
-        <v>24.666666666666668</v>
-      </c>
-      <c r="H6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>1000000</v>
-      </c>
-      <c r="D7">
-        <v>27.4</v>
-      </c>
-      <c r="E7">
-        <v>21.8</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>27.4</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>21.8</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>1500000</v>
-      </c>
-      <c r="D8">
-        <v>40.200000000000003</v>
-      </c>
-      <c r="E8">
-        <v>29.5</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>26.8</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="1"/>
-        <v>19.666666666666668</v>
-      </c>
-      <c r="H8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>2000000</v>
-      </c>
-      <c r="D9">
-        <v>55.8</v>
-      </c>
-      <c r="E9">
-        <v>37.6</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>27.9</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
-        <v>18.8</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>4000000</v>
-      </c>
-      <c r="D10">
-        <v>113</v>
-      </c>
-      <c r="E10">
-        <v>62</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>28.25</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="1"/>
-        <v>15.5</v>
+    <row r="4" spans="1:10" s="27" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="26">
+        <v>262713</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="26">
+        <v>245</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="26">
+        <v>3</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="26">
+        <v>1004570</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="26">
+        <v>71654</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="26">
+        <v>29216</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
2.5 : Détermination de l'unité de energy_100g presque terminé, en utilisant un modèle knn. Reste un petit problème pour une option cat_median censée permettre de remplir les NaN par la médiane de la catégorie. - 2.6 : Avancé dans le calcul du nutriscore. NB : réuni P3_Cleaning à nouveau en un seul fichier
</commit_message>
<xml_diff>
--- a/energy data.xlsx
+++ b/energy data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -778,7 +778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1128,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>